<commit_message>
Made PMS respect footprint differences
</commit_message>
<xml_diff>
--- a/Motherboard Assembly/Project Outputs for Motherboard Assembly/Motherboard Assembly.xlsx
+++ b/Motherboard Assembly/Project Outputs for Motherboard Assembly/Motherboard Assembly.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pr3de\Documents\MASA\2020-21-PCBs\Motherboard Assembly\Project Outputs for Motherboard Assembly\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5C93D04A-4D93-4092-8075-6FDF0FB0C46A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1BE5B086-6EDD-415E-B84F-DEBA801FB26A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{D24AC2E5-4D69-4F47-9D68-7C6EF3866D9C}"/>
+    <workbookView xWindow="7200" yWindow="3405" windowWidth="21600" windowHeight="11385" xr2:uid="{D24AC2E5-4D69-4F47-9D68-7C6EF3866D9C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>